<commit_message>
Update of supplementary materials 01-19-2026
</commit_message>
<xml_diff>
--- a/Effort_Matrix.xlsx
+++ b/Effort_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vlad/Desktop/Proyectos/Activos/Calakmul-Mamíferos/Github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D9028E5-183C-934C-9B2D-B3897A91341F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E3CCD0-96A6-1F4E-91A9-A65434B8A684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{D858C264-1B48-0F48-A4DA-3E852D58CE97}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$2387</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$2384</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Outside</t>
   </si>
@@ -50,15 +50,6 @@
   </si>
   <si>
     <t>Effort</t>
-  </si>
-  <si>
-    <t>RBC</t>
-  </si>
-  <si>
-    <t>Matriz</t>
-  </si>
-  <si>
-    <t>Effort per year</t>
   </si>
   <si>
     <t>Start</t>
@@ -443,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E87011-284D-594A-8AB0-0E4B3C12794E}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,7 +479,7 @@
         <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H2" s="3">
         <v>42459</v>
@@ -511,7 +502,7 @@
         <v>67</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H3" s="3">
         <v>44718</v>
@@ -587,84 +578,6 @@
         <v>701</v>
       </c>
       <c r="E8">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G10" s="1">
-        <v>2021</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>740</v>
-      </c>
-      <c r="C11">
-        <v>347</v>
-      </c>
-      <c r="D11">
-        <v>134</v>
-      </c>
-      <c r="E11">
-        <v>2155</v>
-      </c>
-      <c r="F11">
-        <v>1919</v>
-      </c>
-      <c r="G11">
-        <v>1354</v>
-      </c>
-      <c r="H11">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>67</v>
-      </c>
-      <c r="D12">
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <v>173</v>
-      </c>
-      <c r="F12">
-        <v>89</v>
-      </c>
-      <c r="G12">
-        <v>147</v>
-      </c>
-      <c r="H12">
         <v>362</v>
       </c>
     </row>

</xml_diff>